<commit_message>
added standup meeting scripts
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="6495" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14880" windowHeight="6495" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="IterationOptions" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -540,7 +541,7 @@
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -735,7 +736,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>8</v>
@@ -769,7 +770,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Select the Execution True for all test cases in Runmanager.xlsx
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="6060" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14010" windowHeight="6060" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">Verify Jira Login </t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>TC41_VerifyAssigneIssue</t>
   </si>
   <si>
@@ -175,6 +172,39 @@
   </si>
   <si>
     <t>Verify Create Issue for user add sprint</t>
+  </si>
+  <si>
+    <t>TC61_VerifyStandupMeetingAddWorklogNoHindrancesNoBamdwidth</t>
+  </si>
+  <si>
+    <t>Verify standup meeting</t>
+  </si>
+  <si>
+    <t>TC54_VerifyCreateIssueForUserNoSprint</t>
+  </si>
+  <si>
+    <t>Verify create issues for user no sprint</t>
+  </si>
+  <si>
+    <t>TC62_VerifyStandupMeetingNoWorklogNoHindrancesNoBamdwidth</t>
+  </si>
+  <si>
+    <t>TC63_VerifyStandupMeetingAddWorklogNoHindrancesAddBandwidth</t>
+  </si>
+  <si>
+    <t>TC64_VerifyStandupMeetingNoWorklogNoHindrancesAddBandwidth</t>
+  </si>
+  <si>
+    <t>TC65_VerifyStandupMeetingAddWorklogAddHindrancesNoBandwidth</t>
+  </si>
+  <si>
+    <t>TC66_VerifyStandupMeetingNoWorklogAddHindrancesNoBandwidth</t>
+  </si>
+  <si>
+    <t>TC67_VerifyStandupMeetingAddWorklogAddHindrancesAddBandwidth</t>
+  </si>
+  <si>
+    <t>TC68_VerifyStandupMeetingNoWorklogAddHindrancesAddBandwidth</t>
   </si>
 </sst>
 </file>
@@ -243,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -268,6 +298,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK32"/>
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -617,7 +648,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -634,7 +665,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -642,16 +673,16 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -659,16 +690,16 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -676,16 +707,16 @@
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
@@ -693,16 +724,16 @@
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -710,16 +741,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
@@ -727,16 +758,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -744,16 +775,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -761,16 +792,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
@@ -778,10 +809,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="9" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -795,16 +826,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -812,16 +843,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
@@ -829,16 +860,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
@@ -846,16 +877,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
@@ -863,16 +894,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
@@ -880,16 +911,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>8</v>
@@ -897,98 +928,190 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="8"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="8"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
+      <c r="A24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="8"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
+      <c r="A27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
+      <c r="A28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="4"/>
@@ -1005,17 +1128,22 @@
       <c r="D32" s="5"/>
       <c r="E32" s="4"/>
     </row>
+    <row r="33" spans="3:5">
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33">
       <formula1>"firefox,internetexplorer,chrome"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D33">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E32">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E33">
       <formula1>"All Iterations,1-2,1-3,1-4,1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>